<commit_message>
Actualización automática de fotos y catálogo
</commit_message>
<xml_diff>
--- a/catalogo.xlsx
+++ b/catalogo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
   <si>
     <t>nombre</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>Paris</t>
+  </si>
+  <si>
+    <t>Prueba</t>
   </si>
   <si>
     <t>tipos</t>
@@ -296,8 +299,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0&quot;€&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -331,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -343,6 +347,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1482,10 +1489,18 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="5"/>
+      <c r="A40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="5">
+        <v>12.0</v>
+      </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1496,7 +1511,7 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="6"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -1507,7 +1522,7 @@
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="6"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1518,7 +1533,7 @@
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="6"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1529,7 +1544,7 @@
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="6"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -1540,7 +1555,7 @@
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="6"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -1551,7 +1566,7 @@
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="6"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1562,7 +1577,7 @@
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="5"/>
+      <c r="D47" s="6"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -1573,7 +1588,7 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="6"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -1583,8 +1598,8 @@
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="5"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="6"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -1593,9 +1608,9 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="2"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="5"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="6"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -1604,9 +1619,9 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="2"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="5"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="6"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -1615,9 +1630,9 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="2"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="5"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="6"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -1626,9 +1641,9 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="2"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="5"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="6"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -1637,9 +1652,9 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="2"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="5"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="6"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -1648,9 +1663,9 @@
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="2"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="5"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="6"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2651,7 +2666,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Actualización automática de catálogo y fotos
</commit_message>
<xml_diff>
--- a/catalogo.xlsx
+++ b/catalogo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
   <si>
     <t>nombre</t>
   </si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t>Paris</t>
-  </si>
-  <si>
-    <t>Prueba</t>
   </si>
   <si>
     <t>tipos</t>
@@ -1490,18 +1487,9 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="5">
-        <v>12.0</v>
-      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2633,7 +2621,7 @@
     <row r="1013" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B49">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B39 B41:B49">
       <formula1>datos!$A$2:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C48">
@@ -2667,7 +2655,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>

</xml_diff>